<commit_message>
TestNg File added for Seller flow
</commit_message>
<xml_diff>
--- a/CheckLot/CheckLot2.xlsx
+++ b/CheckLot/CheckLot2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\podommeti\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shbiradar\git\CheckLot\CheckLot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187B081E-8F33-45BC-A699-80F7722DC2FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279CF4FE-1F2D-4231-A0E7-1C87DBE66F4A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,21 +182,6 @@
     <t>Title only assignment closed</t>
   </si>
   <si>
-    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =10 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 10</t>
-  </si>
-  <si>
-    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =15 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 10</t>
-  </si>
-  <si>
-    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =20 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 10</t>
-  </si>
-  <si>
-    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =28 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 10</t>
-  </si>
-  <si>
-    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =28 AND EW_TS03 IS NOT NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 10</t>
-  </si>
-  <si>
     <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =30 AND EW_TS03 IS NOT NULL AND EW_TS04 IS NOT NULL ORDER BY LTLOTNBR DESC LIMIT 1</t>
   </si>
   <si>
@@ -249,6 +234,21 @@
   </si>
   <si>
     <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =40 AND LTXTLMMM = 0 AND LTOTLMMM&gt;0  ORDER BY LTLOTNBR DESC LIMIT 1</t>
+  </si>
+  <si>
+    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =28 AND EW_TS03 IS NOT NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 1</t>
+  </si>
+  <si>
+    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =28 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 1</t>
+  </si>
+  <si>
+    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =20 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 1</t>
+  </si>
+  <si>
+    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =15 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 1</t>
+  </si>
+  <si>
+    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =10 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 1</t>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +689,7 @@
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="7" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="7" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -723,7 +723,7 @@
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="7" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -740,7 +740,7 @@
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="7" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -757,7 +757,7 @@
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="7" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -774,7 +774,7 @@
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -791,7 +791,7 @@
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -808,7 +808,7 @@
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -825,7 +825,7 @@
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -842,7 +842,7 @@
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -876,7 +876,7 @@
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -893,7 +893,7 @@
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -910,7 +910,7 @@
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -927,7 +927,7 @@
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -944,7 +944,7 @@
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -978,7 +978,7 @@
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -995,7 +995,7 @@
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1012,7 +1012,7 @@
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1029,7 +1029,7 @@
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TestNg File added for Seller flow (#2)
Co-authored-by: sharanbiradar <sharanabasava.biradar@copart.com>
</commit_message>
<xml_diff>
--- a/CheckLot/CheckLot2.xlsx
+++ b/CheckLot/CheckLot2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\podommeti\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shbiradar\git\CheckLot\CheckLot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187B081E-8F33-45BC-A699-80F7722DC2FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279CF4FE-1F2D-4231-A0E7-1C87DBE66F4A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,21 +182,6 @@
     <t>Title only assignment closed</t>
   </si>
   <si>
-    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =10 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 10</t>
-  </si>
-  <si>
-    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =15 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 10</t>
-  </si>
-  <si>
-    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =20 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 10</t>
-  </si>
-  <si>
-    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =28 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 10</t>
-  </si>
-  <si>
-    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =28 AND EW_TS03 IS NOT NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 10</t>
-  </si>
-  <si>
     <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =30 AND EW_TS03 IS NOT NULL AND EW_TS04 IS NOT NULL ORDER BY LTLOTNBR DESC LIMIT 1</t>
   </si>
   <si>
@@ -249,6 +234,21 @@
   </si>
   <si>
     <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =40 AND LTXTLMMM = 0 AND LTOTLMMM&gt;0  ORDER BY LTLOTNBR DESC LIMIT 1</t>
+  </si>
+  <si>
+    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =28 AND EW_TS03 IS NOT NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 1</t>
+  </si>
+  <si>
+    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =28 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 1</t>
+  </si>
+  <si>
+    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =20 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 1</t>
+  </si>
+  <si>
+    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =15 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 1</t>
+  </si>
+  <si>
+    <t>SELECT LTLOTNBR, LTSLRNBR FROM MISPRDDB.LOTLT a JOIN MISPRDDB.LOTLTNEW b ON a.LTLOTNBR = b.LOT_NUMBER WHERE LTLOTSTG =10 AND EW_TS03 IS NULL AND EW_TS04 is NULL ORDER BY LTLOTNBR DESC LIMIT 1</t>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +689,7 @@
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="7" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -706,7 +706,7 @@
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="7" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -723,7 +723,7 @@
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="7" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -740,7 +740,7 @@
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="7" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -757,7 +757,7 @@
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="7" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -774,7 +774,7 @@
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -791,7 +791,7 @@
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -808,7 +808,7 @@
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -825,7 +825,7 @@
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -842,7 +842,7 @@
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -876,7 +876,7 @@
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -893,7 +893,7 @@
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -910,7 +910,7 @@
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -927,7 +927,7 @@
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -944,7 +944,7 @@
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -961,7 +961,7 @@
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -978,7 +978,7 @@
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -995,7 +995,7 @@
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1012,7 +1012,7 @@
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1029,7 +1029,7 @@
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="7" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>